<commit_message>
added assembly notes for Teensy
</commit_message>
<xml_diff>
--- a/PCB/stimjim_SeeedStudioAssembly_BOM.xlsx
+++ b/PCB/stimjim_SeeedStudioAssembly_BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="148">
   <si>
     <t xml:space="preserve">Designator</t>
   </si>
@@ -46,6 +46,9 @@
     <t xml:space="preserve">Total cost</t>
   </si>
   <si>
+    <t xml:space="preserve">Assembly notes</t>
+  </si>
+  <si>
     <t xml:space="preserve">C26,C27,C31,C32,C34,C35,C38,C39,C42,C41,C2,C7,C6,C1,C13,C43,C44,C18,C20,C9,C14,C16,C17,C45,C46,C21,C19,C48,C49,C47,C50,C23,C24,C22,C25,C11</t>
   </si>
   <si>
@@ -280,6 +283,9 @@
     <t xml:space="preserve">Teensy3.5</t>
   </si>
   <si>
+    <t xml:space="preserve">After soldering male pins onto this part, it should be inserted into the female headers on the board (next line)</t>
+  </si>
+  <si>
     <t xml:space="preserve">PPTC241LFBN-RC</t>
   </si>
   <si>
@@ -292,6 +298,9 @@
     <t xml:space="preserve">Female headers</t>
   </si>
   <si>
+    <t xml:space="preserve">These should be soldered onto the topside of the board at location U1.</t>
+  </si>
+  <si>
     <t xml:space="preserve">PREC024SAAN-RC</t>
   </si>
   <si>
@@ -302,6 +311,9 @@
   </si>
   <si>
     <t xml:space="preserve">male pin headers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These should be soldered onto the bottom side of the Teensy (MPN DEV-14055)</t>
   </si>
   <si>
     <t xml:space="preserve">U10,U21</t>
@@ -722,14 +734,14 @@
   <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
+      <selection pane="topLeft" activeCell="J20" activeCellId="0" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="51.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="20.14"/>
@@ -763,25 +775,28 @@
       <c r="I1" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>36</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>0.038</v>
@@ -793,22 +808,22 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="4" t="n">
         <v>6</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>0.4</v>
@@ -820,22 +835,22 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" s="4" t="n">
         <v>10</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>0.1</v>
@@ -847,22 +862,22 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H5" s="7" t="n">
         <v>0.92</v>
@@ -874,22 +889,22 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>0.64</v>
@@ -901,22 +916,22 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C7" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>0.48</v>
@@ -928,22 +943,22 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C8" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H8" s="1" t="n">
         <v>1.12</v>
@@ -955,7 +970,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B9" s="3" t="n">
         <v>731375003</v>
@@ -964,13 +979,13 @@
         <v>4</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F9" s="3" t="n">
         <v>731375003</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>1.48</v>
@@ -982,22 +997,22 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C10" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>0.11</v>
@@ -1009,22 +1024,22 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C11" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H11" s="0" t="n">
         <v>0.11</v>
@@ -1036,19 +1051,19 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C12" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G12" s="3" t="n">
         <v>200</v>
@@ -1064,22 +1079,22 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C13" s="10" t="n">
         <v>4</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H13" s="0" t="n">
         <v>0.35</v>
@@ -1091,22 +1106,22 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C14" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H14" s="0" t="n">
         <v>0.3</v>
@@ -1118,22 +1133,22 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C15" s="4" t="n">
         <v>4</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>0.8</v>
@@ -1145,22 +1160,22 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C16" s="10" t="n">
         <v>2</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H16" s="0" t="n">
         <v>0.35</v>
@@ -1172,19 +1187,19 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C17" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G17" s="3" t="n">
         <v>100</v>
@@ -1199,22 +1214,22 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C18" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H18" s="0" t="n">
         <v>0.23</v>
@@ -1226,22 +1241,22 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C19" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H19" s="0" t="n">
         <v>26.25</v>
@@ -1250,25 +1265,28 @@
         <f aca="false">H19*C19</f>
         <v>26.25</v>
       </c>
+      <c r="J19" s="0" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C20" s="10" t="n">
         <v>2</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H20" s="0" t="n">
         <v>1.37</v>
@@ -1277,25 +1295,28 @@
         <f aca="false">H20*C20</f>
         <v>2.74</v>
       </c>
+      <c r="J20" s="0" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C21" s="10" t="n">
         <v>2</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="H21" s="0" t="n">
         <v>0.46</v>
@@ -1304,25 +1325,28 @@
         <f aca="false">H21*C21</f>
         <v>0.92</v>
       </c>
+      <c r="J21" s="0" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C22" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="H22" s="0" t="n">
         <v>7.4</v>
@@ -1339,22 +1363,22 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C23" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="H23" s="0" t="n">
         <v>4.44</v>
@@ -1366,22 +1390,22 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C24" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D24" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="F24" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="G24" s="3" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="H24" s="1" t="n">
         <v>3.76</v>
@@ -1394,22 +1418,22 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C25" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H25" s="0" t="n">
         <v>15.96</v>
@@ -1421,22 +1445,22 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C26" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="H26" s="0" t="n">
         <v>7.84</v>
@@ -1448,22 +1472,22 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C27" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="H27" s="0" t="n">
         <v>1.76</v>
@@ -1475,22 +1499,22 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C28" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="H28" s="0" t="n">
         <v>11.21</v>
@@ -1502,22 +1526,22 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C29" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="H29" s="0" t="n">
         <v>1.6</v>
@@ -1529,22 +1553,22 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C30" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="H30" s="0" t="n">
         <v>2.81</v>
@@ -1556,22 +1580,22 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C31" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="H31" s="0" t="n">
         <v>2.43</v>
@@ -1584,22 +1608,22 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C32" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="H32" s="0" t="n">
         <v>0.48</v>

</xml_diff>